<commit_message>
ajustando parametros de filtros
</commit_message>
<xml_diff>
--- a/modelo planilha/PEP a PEP - Incorridos - Modelo.xlsx
+++ b/modelo planilha/PEP a PEP - Incorridos - Modelo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Bot Fabricio\modelo planilha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renan.oliveira\Desktop\Scripts\gerador_incorridos\modelo planilha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7819E55-2238-4297-9205-10A07791D7F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEEED3B-1284-467F-BE07-D4AF604B575B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{FF0CDEF6-1121-4D75-9F35-6CA55A6AF6BA}"/>
+    <workbookView xWindow="0" yWindow="1860" windowWidth="17160" windowHeight="8175" xr2:uid="{FF0CDEF6-1121-4D75-9F35-6CA55A6AF6BA}"/>
   </bookViews>
   <sheets>
     <sheet name="PEP A PEP" sheetId="2" r:id="rId1"/>
@@ -156,9 +156,6 @@
     <t>Instalações Provisórias</t>
   </si>
   <si>
-    <t>POCRCIIPR</t>
-  </si>
-  <si>
     <t>Sistema de Proteção</t>
   </si>
   <si>
@@ -385,6 +382,9 @@
   </si>
   <si>
     <t>m023</t>
+  </si>
+  <si>
+    <t>POCRCIPR</t>
   </si>
 </sst>
 </file>
@@ -1953,12 +1953,12 @@
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
     <cellStyle name="Vírgula 3" xfId="3" xr:uid="{0F77B90D-75AB-4E7E-BEDD-BBA6DBA0BBA0}"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="31">
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i/>
-        <color rgb="FFC00000"/>
+        <color theme="9" tint="-0.24994659260841701"/>
       </font>
     </dxf>
     <dxf>
@@ -1966,55 +1966,6 @@
         <b val="0"/>
         <i/>
         <color rgb="FFFF5757"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color rgb="FFFF5757"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color rgb="FFFF5757"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color rgb="FFFF5757"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color rgb="FFFF9393"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color rgb="FFFF5757"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="9" tint="-0.24994659260841701"/>
       </font>
     </dxf>
     <dxf>
@@ -2049,6 +2000,13 @@
       <font>
         <b/>
         <i/>
+        <color rgb="FFFF5757"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
         <color theme="9" tint="-0.24994659260841701"/>
       </font>
     </dxf>
@@ -2056,7 +2014,7 @@
       <font>
         <b/>
         <i/>
-        <color rgb="FFFF5757"/>
+        <color theme="9" tint="0.59996337778862885"/>
       </font>
     </dxf>
     <dxf>
@@ -2064,13 +2022,6 @@
         <b/>
         <i/>
         <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color theme="9" tint="0.59996337778862885"/>
       </font>
     </dxf>
     <dxf>
@@ -2091,6 +2042,13 @@
       <font>
         <b/>
         <i/>
+        <color rgb="FFFF5757"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
         <color theme="9" tint="-0.24994659260841701"/>
       </font>
     </dxf>
@@ -2098,7 +2056,7 @@
       <font>
         <b/>
         <i/>
-        <color rgb="FFFF5757"/>
+        <color rgb="FFFF9393"/>
       </font>
     </dxf>
     <dxf>
@@ -2106,13 +2064,6 @@
         <b/>
         <i/>
         <color rgb="FFA9D08E"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <color rgb="FFFF9393"/>
       </font>
     </dxf>
     <dxf>
@@ -2141,6 +2092,20 @@
         <b/>
         <i/>
         <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color rgb="FFFF5757"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <color rgb="FFFF9393"/>
       </font>
     </dxf>
     <dxf>
@@ -2536,10 +2501,10 @@
   <dimension ref="B1:N116"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="12" ySplit="7" topLeftCell="M8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="7" topLeftCell="M16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -2566,7 +2531,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="135" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2918,10 +2883,10 @@
       <c r="B19" s="42"/>
       <c r="C19" s="193"/>
       <c r="D19" s="157" t="s">
+        <v>104</v>
+      </c>
+      <c r="E19" s="159" t="s">
         <v>28</v>
-      </c>
-      <c r="E19" s="159" t="s">
-        <v>29</v>
       </c>
       <c r="F19" s="45"/>
       <c r="G19" s="172"/>
@@ -2943,10 +2908,10 @@
       <c r="B20" s="42"/>
       <c r="C20" s="193"/>
       <c r="D20" s="157" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="159" t="s">
         <v>30</v>
-      </c>
-      <c r="E20" s="159" t="s">
-        <v>31</v>
       </c>
       <c r="F20" s="45"/>
       <c r="G20" s="172"/>
@@ -2968,10 +2933,10 @@
       <c r="B21" s="42"/>
       <c r="C21" s="193"/>
       <c r="D21" s="157" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="159" t="s">
         <v>32</v>
-      </c>
-      <c r="E21" s="159" t="s">
-        <v>33</v>
       </c>
       <c r="F21" s="45"/>
       <c r="G21" s="172"/>
@@ -2993,10 +2958,10 @@
       <c r="B22" s="42"/>
       <c r="C22" s="193"/>
       <c r="D22" s="157" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="159" t="s">
         <v>34</v>
-      </c>
-      <c r="E22" s="159" t="s">
-        <v>35</v>
       </c>
       <c r="F22" s="45"/>
       <c r="G22" s="172"/>
@@ -3018,10 +2983,10 @@
       <c r="B23" s="42"/>
       <c r="C23" s="193"/>
       <c r="D23" s="155" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="156" t="s">
         <v>36</v>
-      </c>
-      <c r="E23" s="156" t="s">
-        <v>37</v>
       </c>
       <c r="F23" s="45"/>
       <c r="G23" s="49">
@@ -3049,10 +3014,10 @@
       <c r="B24" s="42"/>
       <c r="C24" s="193"/>
       <c r="D24" s="157" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="159" t="s">
         <v>38</v>
-      </c>
-      <c r="E24" s="159" t="s">
-        <v>39</v>
       </c>
       <c r="G24" s="172"/>
       <c r="H24" s="54">
@@ -3074,10 +3039,10 @@
       <c r="B25" s="42"/>
       <c r="C25" s="193"/>
       <c r="D25" s="157" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="159" t="s">
         <v>40</v>
-      </c>
-      <c r="E25" s="159" t="s">
-        <v>41</v>
       </c>
       <c r="G25" s="172"/>
       <c r="H25" s="54">
@@ -3099,10 +3064,10 @@
       <c r="B26" s="42"/>
       <c r="C26" s="193"/>
       <c r="D26" s="157" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="159" t="s">
         <v>42</v>
-      </c>
-      <c r="E26" s="159" t="s">
-        <v>43</v>
       </c>
       <c r="G26" s="172"/>
       <c r="H26" s="54">
@@ -3124,10 +3089,10 @@
       <c r="B27" s="42"/>
       <c r="C27" s="193"/>
       <c r="D27" s="157" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="159" t="s">
         <v>44</v>
-      </c>
-      <c r="E27" s="159" t="s">
-        <v>45</v>
       </c>
       <c r="G27" s="172"/>
       <c r="H27" s="54">
@@ -3149,10 +3114,10 @@
       <c r="B28" s="42"/>
       <c r="C28" s="193"/>
       <c r="D28" s="157" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" s="159" t="s">
         <v>46</v>
-      </c>
-      <c r="E28" s="159" t="s">
-        <v>47</v>
       </c>
       <c r="G28" s="172"/>
       <c r="H28" s="54">
@@ -3174,10 +3139,10 @@
       <c r="B29" s="42"/>
       <c r="C29" s="193"/>
       <c r="D29" s="157" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="159" t="s">
         <v>48</v>
-      </c>
-      <c r="E29" s="159" t="s">
-        <v>49</v>
       </c>
       <c r="G29" s="172"/>
       <c r="H29" s="54">
@@ -3199,10 +3164,10 @@
       <c r="B30" s="42"/>
       <c r="C30" s="193"/>
       <c r="D30" s="157" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="159" t="s">
         <v>50</v>
-      </c>
-      <c r="E30" s="159" t="s">
-        <v>51</v>
       </c>
       <c r="G30" s="172"/>
       <c r="H30" s="54">
@@ -3224,10 +3189,10 @@
       <c r="B31" s="42"/>
       <c r="C31" s="193"/>
       <c r="D31" s="157" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="159" t="s">
         <v>52</v>
-      </c>
-      <c r="E31" s="159" t="s">
-        <v>53</v>
       </c>
       <c r="G31" s="172"/>
       <c r="H31" s="54">
@@ -3249,10 +3214,10 @@
       <c r="B32" s="42"/>
       <c r="C32" s="193"/>
       <c r="D32" s="157" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" s="159" t="s">
         <v>54</v>
-      </c>
-      <c r="E32" s="159" t="s">
-        <v>55</v>
       </c>
       <c r="G32" s="172"/>
       <c r="H32" s="54">
@@ -3274,10 +3239,10 @@
       <c r="B33" s="42"/>
       <c r="C33" s="193"/>
       <c r="D33" s="157" t="s">
+        <v>55</v>
+      </c>
+      <c r="E33" s="159" t="s">
         <v>56</v>
-      </c>
-      <c r="E33" s="159" t="s">
-        <v>57</v>
       </c>
       <c r="G33" s="172"/>
       <c r="H33" s="54">
@@ -3299,10 +3264,10 @@
       <c r="B34" s="42"/>
       <c r="C34" s="193"/>
       <c r="D34" s="157" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34" s="159" t="s">
         <v>58</v>
-      </c>
-      <c r="E34" s="159" t="s">
-        <v>59</v>
       </c>
       <c r="G34" s="172"/>
       <c r="H34" s="54">
@@ -3324,10 +3289,10 @@
       <c r="B35" s="42"/>
       <c r="C35" s="193"/>
       <c r="D35" s="157" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" s="159" t="s">
         <v>60</v>
-      </c>
-      <c r="E35" s="159" t="s">
-        <v>61</v>
       </c>
       <c r="G35" s="172"/>
       <c r="H35" s="54">
@@ -3349,10 +3314,10 @@
       <c r="B36" s="42"/>
       <c r="C36" s="193"/>
       <c r="D36" s="157" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" s="159" t="s">
         <v>62</v>
-      </c>
-      <c r="E36" s="159" t="s">
-        <v>63</v>
       </c>
       <c r="G36" s="172"/>
       <c r="H36" s="54">
@@ -3374,10 +3339,10 @@
       <c r="B37" s="42"/>
       <c r="C37" s="193"/>
       <c r="D37" s="157" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" s="159" t="s">
         <v>64</v>
-      </c>
-      <c r="E37" s="159" t="s">
-        <v>65</v>
       </c>
       <c r="G37" s="172"/>
       <c r="H37" s="54">
@@ -3399,10 +3364,10 @@
       <c r="B38" s="42"/>
       <c r="C38" s="193"/>
       <c r="D38" s="157" t="s">
+        <v>65</v>
+      </c>
+      <c r="E38" s="159" t="s">
         <v>66</v>
-      </c>
-      <c r="E38" s="159" t="s">
-        <v>67</v>
       </c>
       <c r="G38" s="172"/>
       <c r="H38" s="54">
@@ -3424,10 +3389,10 @@
       <c r="B39" s="42"/>
       <c r="C39" s="193"/>
       <c r="D39" s="157" t="s">
+        <v>67</v>
+      </c>
+      <c r="E39" s="159" t="s">
         <v>68</v>
-      </c>
-      <c r="E39" s="159" t="s">
-        <v>69</v>
       </c>
       <c r="G39" s="172"/>
       <c r="H39" s="54">
@@ -3449,10 +3414,10 @@
       <c r="B40" s="42"/>
       <c r="C40" s="193"/>
       <c r="D40" s="157" t="s">
+        <v>69</v>
+      </c>
+      <c r="E40" s="159" t="s">
         <v>70</v>
-      </c>
-      <c r="E40" s="159" t="s">
-        <v>71</v>
       </c>
       <c r="G40" s="172"/>
       <c r="H40" s="54">
@@ -3474,10 +3439,10 @@
       <c r="B41" s="42"/>
       <c r="C41" s="193"/>
       <c r="D41" s="157" t="s">
+        <v>71</v>
+      </c>
+      <c r="E41" s="159" t="s">
         <v>72</v>
-      </c>
-      <c r="E41" s="159" t="s">
-        <v>73</v>
       </c>
       <c r="G41" s="172"/>
       <c r="H41" s="54">
@@ -3499,10 +3464,10 @@
       <c r="B42" s="42"/>
       <c r="C42" s="193"/>
       <c r="D42" s="157" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42" s="159" t="s">
         <v>74</v>
-      </c>
-      <c r="E42" s="159" t="s">
-        <v>75</v>
       </c>
       <c r="G42" s="172"/>
       <c r="H42" s="54">
@@ -3524,10 +3489,10 @@
       <c r="B43" s="42"/>
       <c r="C43" s="193"/>
       <c r="D43" s="157" t="s">
+        <v>75</v>
+      </c>
+      <c r="E43" s="159" t="s">
         <v>76</v>
-      </c>
-      <c r="E43" s="159" t="s">
-        <v>77</v>
       </c>
       <c r="G43" s="172"/>
       <c r="H43" s="54">
@@ -3549,10 +3514,10 @@
       <c r="B44" s="42"/>
       <c r="C44" s="193"/>
       <c r="D44" s="157" t="s">
+        <v>77</v>
+      </c>
+      <c r="E44" s="159" t="s">
         <v>78</v>
-      </c>
-      <c r="E44" s="159" t="s">
-        <v>79</v>
       </c>
       <c r="G44" s="172"/>
       <c r="H44" s="54">
@@ -3574,10 +3539,10 @@
       <c r="B45" s="42"/>
       <c r="C45" s="193"/>
       <c r="D45" s="157" t="s">
+        <v>79</v>
+      </c>
+      <c r="E45" s="159" t="s">
         <v>80</v>
-      </c>
-      <c r="E45" s="159" t="s">
-        <v>81</v>
       </c>
       <c r="G45" s="172"/>
       <c r="H45" s="54">
@@ -3599,7 +3564,7 @@
       <c r="B46" s="42"/>
       <c r="C46" s="193"/>
       <c r="D46" s="157" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E46" s="177"/>
       <c r="G46" s="172"/>
@@ -3622,7 +3587,7 @@
       <c r="B47" s="42"/>
       <c r="C47" s="193"/>
       <c r="D47" s="157" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E47" s="177"/>
       <c r="G47" s="172"/>
@@ -3642,7 +3607,7 @@
       <c r="B48" s="42"/>
       <c r="C48" s="193"/>
       <c r="D48" s="157" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E48" s="177"/>
       <c r="G48" s="172"/>
@@ -3662,7 +3627,7 @@
       <c r="B49" s="42"/>
       <c r="C49" s="193"/>
       <c r="D49" s="157" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E49" s="177"/>
       <c r="G49" s="172"/>
@@ -3682,7 +3647,7 @@
       <c r="B50" s="42"/>
       <c r="C50" s="193"/>
       <c r="D50" s="157" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E50" s="177"/>
       <c r="G50" s="172"/>
@@ -3702,7 +3667,7 @@
       <c r="B51" s="42"/>
       <c r="C51" s="193"/>
       <c r="D51" s="157" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E51" s="177"/>
       <c r="G51" s="172"/>
@@ -3722,7 +3687,7 @@
       <c r="B52" s="42"/>
       <c r="C52" s="193"/>
       <c r="D52" s="157" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E52" s="177"/>
       <c r="G52" s="172"/>
@@ -3742,7 +3707,7 @@
       <c r="B53" s="42"/>
       <c r="C53" s="193"/>
       <c r="D53" s="157" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E53" s="177"/>
       <c r="G53" s="172"/>
@@ -3762,10 +3727,10 @@
       <c r="B54" s="42"/>
       <c r="C54" s="193"/>
       <c r="D54" s="153" t="s">
+        <v>89</v>
+      </c>
+      <c r="E54" s="154" t="s">
         <v>90</v>
-      </c>
-      <c r="E54" s="154" t="s">
-        <v>91</v>
       </c>
       <c r="G54" s="169"/>
       <c r="H54" s="41">
@@ -3784,10 +3749,10 @@
       <c r="B55" s="42"/>
       <c r="C55" s="193"/>
       <c r="D55" s="153" t="s">
+        <v>91</v>
+      </c>
+      <c r="E55" s="154" t="s">
         <v>92</v>
-      </c>
-      <c r="E55" s="154" t="s">
-        <v>93</v>
       </c>
       <c r="G55" s="169"/>
       <c r="H55" s="41">
@@ -3806,10 +3771,10 @@
       <c r="B56" s="42"/>
       <c r="C56" s="193"/>
       <c r="D56" s="160" t="s">
+        <v>93</v>
+      </c>
+      <c r="E56" s="161" t="s">
         <v>94</v>
-      </c>
-      <c r="E56" s="161" t="s">
-        <v>95</v>
       </c>
       <c r="G56" s="150">
         <f>SUM(G57:G59)</f>
@@ -3831,10 +3796,10 @@
       <c r="B57" s="42"/>
       <c r="C57" s="193"/>
       <c r="D57" s="155" t="s">
+        <v>95</v>
+      </c>
+      <c r="E57" s="156" t="s">
         <v>96</v>
-      </c>
-      <c r="E57" s="156" t="s">
-        <v>97</v>
       </c>
       <c r="G57" s="170"/>
       <c r="H57" s="164">
@@ -3853,10 +3818,10 @@
       <c r="B58" s="42"/>
       <c r="C58" s="193"/>
       <c r="D58" s="155" t="s">
+        <v>97</v>
+      </c>
+      <c r="E58" s="156" t="s">
         <v>98</v>
-      </c>
-      <c r="E58" s="156" t="s">
-        <v>99</v>
       </c>
       <c r="G58" s="170"/>
       <c r="H58" s="164">
@@ -3875,10 +3840,10 @@
       <c r="B59" s="42"/>
       <c r="C59" s="194"/>
       <c r="D59" s="162" t="s">
+        <v>99</v>
+      </c>
+      <c r="E59" s="163" t="s">
         <v>100</v>
-      </c>
-      <c r="E59" s="163" t="s">
-        <v>101</v>
       </c>
       <c r="G59" s="171"/>
       <c r="H59" s="166">
@@ -3932,7 +3897,7 @@
       <c r="D63" s="196"/>
       <c r="E63" s="84"/>
       <c r="G63" s="85" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H63" s="86"/>
       <c r="I63" s="87"/>
@@ -3961,7 +3926,7 @@
     <row r="66" spans="2:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="94"/>
       <c r="C66" s="202" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D66" s="95" t="str">
         <f>D10</f>
@@ -4241,7 +4206,7 @@
       <c r="C75" s="203"/>
       <c r="D75" s="184" t="str">
         <f t="shared" si="6"/>
-        <v>POCRCIIPR</v>
+        <v>POCRCIPR</v>
       </c>
       <c r="E75" s="185" t="str">
         <f t="shared" si="7"/>
@@ -5475,168 +5440,143 @@
     <mergeCell ref="G64:I64"/>
     <mergeCell ref="C66:C115"/>
   </mergeCells>
-  <conditionalFormatting sqref="D11:E14 G11:G14 D54:E56 G54:G59 I54:I59 I11:I14">
-    <cfRule type="expression" dxfId="35" priority="42">
+  <conditionalFormatting sqref="D11:E14 D54:E56">
+    <cfRule type="expression" dxfId="30" priority="42">
       <formula>$H11&gt;$G11</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16:E22 G16:G22 D24:E53 G24:G53 I24:I53 I16:I22">
-    <cfRule type="expression" dxfId="34" priority="41">
+  <conditionalFormatting sqref="D16:E22 D24:E53">
+    <cfRule type="expression" dxfId="29" priority="41">
       <formula>$H16&gt;$G16</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D57:E59">
-    <cfRule type="expression" dxfId="33" priority="32">
+    <cfRule type="expression" dxfId="28" priority="32">
       <formula>$H57&gt;$G57</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D67:E70">
-    <cfRule type="expression" dxfId="32" priority="27">
+    <cfRule type="expression" dxfId="27" priority="27">
       <formula>$H67&gt;$G67</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D72:E78">
-    <cfRule type="expression" dxfId="31" priority="24">
+    <cfRule type="expression" dxfId="26" priority="24">
       <formula>$H72&gt;$G72</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D80:E109">
-    <cfRule type="expression" dxfId="30" priority="25">
+    <cfRule type="expression" dxfId="25" priority="25">
       <formula>$H80&gt;$G80</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D110:E112">
-    <cfRule type="expression" dxfId="29" priority="26">
+    <cfRule type="expression" dxfId="24" priority="26">
       <formula>$H110&gt;$G110</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15:G15 D23:G23 I23 I15">
-    <cfRule type="expression" dxfId="28" priority="43">
+  <conditionalFormatting sqref="D15:I15 D23:I23">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>$H15&gt;$G15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F71 F79">
-    <cfRule type="expression" dxfId="27" priority="29">
+    <cfRule type="expression" dxfId="22" priority="29">
       <formula>$H71&gt;$G71</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G67:G70 I67:I70">
-    <cfRule type="expression" dxfId="26" priority="20">
+  <conditionalFormatting sqref="G11:I14 G54:I59">
+    <cfRule type="expression" dxfId="21" priority="6">
+      <formula>$H11&gt;$G11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G16:I22 G24:I53">
+    <cfRule type="expression" dxfId="20" priority="5">
+      <formula>$H16&gt;$G16</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G67:I70">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>$H67&gt;$G67</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G72:G78 I72:I78">
-    <cfRule type="expression" dxfId="25" priority="23">
+  <conditionalFormatting sqref="G72:I78">
+    <cfRule type="expression" dxfId="18" priority="4">
       <formula>$H72&gt;$G72</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G80:G109 I80:I109">
-    <cfRule type="expression" dxfId="24" priority="22">
+  <conditionalFormatting sqref="G80:I109">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>$H80&gt;$G80</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G110:G112 I110:I112">
-    <cfRule type="expression" dxfId="23" priority="21">
+  <conditionalFormatting sqref="G110:I112">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>$H110&gt;$G110</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14">
-    <cfRule type="expression" dxfId="22" priority="36">
+    <cfRule type="expression" dxfId="15" priority="37">
+      <formula>$L14&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="36">
       <formula>$L14&lt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="37">
-      <formula>$L14&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15 L23">
-    <cfRule type="expression" dxfId="20" priority="38">
+    <cfRule type="expression" dxfId="13" priority="39">
+      <formula>$L15&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="38">
       <formula>$L15&lt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="39">
-      <formula>$L15&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16:L22 L24:L53">
-    <cfRule type="expression" dxfId="18" priority="40">
+    <cfRule type="expression" dxfId="11" priority="40">
       <formula>$L16&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="44">
+    <cfRule type="expression" dxfId="10" priority="44">
       <formula>$L16&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L70">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="9" priority="18">
+      <formula>$L70&lt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="17">
       <formula>$L70&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="15" priority="18">
-      <formula>$L70&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L71">
-    <cfRule type="expression" dxfId="14" priority="11">
+    <cfRule type="expression" dxfId="7" priority="12">
+      <formula>$L71&gt;0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="11">
       <formula>$L71&lt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="12">
-      <formula>$L71&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L72:L78">
-    <cfRule type="expression" dxfId="12" priority="28">
+    <cfRule type="expression" dxfId="5" priority="28">
       <formula>$L72&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="30">
+    <cfRule type="expression" dxfId="4" priority="30">
       <formula>$L72&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L79">
-    <cfRule type="expression" dxfId="10" priority="8">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>$L79&lt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="2" priority="9">
       <formula>$L79&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L80:L109">
-    <cfRule type="expression" dxfId="8" priority="14">
-      <formula>$L80&gt;0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="7" priority="15">
+    <cfRule type="expression" dxfId="1" priority="15">
       <formula>$L80&lt;0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H11:H14 H54:H59">
-    <cfRule type="expression" dxfId="6" priority="6">
-      <formula>$H11&gt;$G11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16:H22 H24:H53">
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>$H16&gt;$G16</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15 H23">
-    <cfRule type="expression" dxfId="4" priority="7">
-      <formula>$H15&gt;$G15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H67:H70">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$H67&gt;$G67</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H72:H78">
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>$H72&gt;$G72</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H80:H109">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>$H80&gt;$G80</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H110:H112">
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>$H110&gt;$G110</formula>
+    <cfRule type="expression" dxfId="0" priority="14">
+      <formula>$L80&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -6284,6 +6224,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A2E69AC71DE3654F97F1183C29BC8261" ma:contentTypeVersion="4" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="882d357326e1215bae8de2ab4e60b4fd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8366f177-07ed-4fc9-be97-e083a2cd3bf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bf3bcc82be21379e317eddbad04fc935" ns2:_="">
     <xsd:import namespace="8366f177-07ed-4fc9-be97-e083a2cd3bf9"/>
@@ -6427,22 +6382,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1858D4A7-903D-4677-86F9-0756F6A8ED4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B81410E7-B7C4-4318-85E7-620A47FED5F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54025C05-9DFC-48B1-AF42-8C333127B25E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6458,21 +6415,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B81410E7-B7C4-4318-85E7-620A47FED5F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1858D4A7-903D-4677-86F9-0756F6A8ED4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adicionando descrição dos codigos SAP
</commit_message>
<xml_diff>
--- a/modelo planilha/PEP a PEP - Incorridos - Modelo.xlsx
+++ b/modelo planilha/PEP a PEP - Incorridos - Modelo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Bot Fabricio\modelo planilha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6DC0DD-8F49-4FAC-8DA2-6F318A3DC2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A316064-A760-45D0-A1CA-D856619585D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23040" yWindow="624" windowWidth="23232" windowHeight="11760" xr2:uid="{FF0CDEF6-1121-4D75-9F35-6CA55A6AF6BA}"/>
+    <workbookView xWindow="-23148" yWindow="-72" windowWidth="23256" windowHeight="12456" xr2:uid="{FF0CDEF6-1121-4D75-9F35-6CA55A6AF6BA}"/>
   </bookViews>
   <sheets>
     <sheet name="PEP A PEP" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t>Obra:</t>
   </si>
@@ -357,9 +357,6 @@
   </si>
   <si>
     <t>MOEDA FORTE</t>
-  </si>
-  <si>
-    <t>m023</t>
   </si>
   <si>
     <t>POCRCIPR</t>
@@ -2485,10 +2482,10 @@
   <dimension ref="B1:N117"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="12" ySplit="7" topLeftCell="M49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="7" topLeftCell="M44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H49" sqref="H49"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -2514,9 +2511,7 @@
       <c r="D2" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="135" t="s">
-        <v>103</v>
-      </c>
+      <c r="E2" s="135"/>
     </row>
     <row r="3" spans="2:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="136"/>
@@ -2860,7 +2855,7 @@
       <c r="B19" s="42"/>
       <c r="C19" s="196"/>
       <c r="D19" s="157" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E19" s="159" t="s">
         <v>28</v>
@@ -2960,10 +2955,10 @@
       <c r="B23" s="42"/>
       <c r="C23" s="196"/>
       <c r="D23" s="157" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" s="159" t="s">
         <v>105</v>
-      </c>
-      <c r="E23" s="159" t="s">
-        <v>106</v>
       </c>
       <c r="F23" s="45"/>
       <c r="G23" s="172"/>
@@ -4372,7 +4367,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H81" s="113">
-        <f t="shared" ref="H81:H112" si="16">SUM(N81:BK81)</f>
+        <f t="shared" ref="H81:H110" si="16">SUM(N81:BK81)</f>
         <v>0</v>
       </c>
       <c r="I81" s="114" t="e">
@@ -6228,9 +6223,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6378,19 +6376,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1858D4A7-903D-4677-86F9-0756F6A8ED4F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B81410E7-B7C4-4318-85E7-620A47FED5F9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6414,9 +6408,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B81410E7-B7C4-4318-85E7-620A47FED5F9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1858D4A7-903D-4677-86F9-0756F6A8ED4F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ajustando formula da planilha
</commit_message>
<xml_diff>
--- a/modelo planilha/PEP a PEP - Incorridos - Modelo.xlsx
+++ b/modelo planilha/PEP a PEP - Incorridos - Modelo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Bot Fabricio\modelo planilha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A316064-A760-45D0-A1CA-D856619585D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBD9B97-692B-4680-9DA9-D284E9C4ACDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-72" windowWidth="23256" windowHeight="12456" xr2:uid="{FF0CDEF6-1121-4D75-9F35-6CA55A6AF6BA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{FF0CDEF6-1121-4D75-9F35-6CA55A6AF6BA}"/>
   </bookViews>
   <sheets>
     <sheet name="PEP A PEP" sheetId="2" r:id="rId1"/>
@@ -2482,10 +2482,10 @@
   <dimension ref="B1:N117"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="12" ySplit="7" topLeftCell="M44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="7" topLeftCell="M49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomRight" activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -2760,7 +2760,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="50">
-        <f>SUM(H16:H22)</f>
+        <f>SUM(H16:XFD16)</f>
         <v>0</v>
       </c>
       <c r="I15" s="51">
@@ -6223,12 +6223,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6376,15 +6373,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B81410E7-B7C4-4318-85E7-620A47FED5F9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1858D4A7-903D-4677-86F9-0756F6A8ED4F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6408,10 +6409,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1858D4A7-903D-4677-86F9-0756F6A8ED4F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B81410E7-B7C4-4318-85E7-620A47FED5F9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>